<commit_message>
bug fixes and virtual env mail created
</commit_message>
<xml_diff>
--- a/rahul/FlaskApp_excel/parsed_email_details.xlsx
+++ b/rahul/FlaskApp_excel/parsed_email_details.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,9 +424,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="64" customWidth="1" min="1" max="1"/>
+    <col width="83" customWidth="1" min="1" max="1"/>
     <col width="39" customWidth="1" min="2" max="2"/>
-    <col width="38" customWidth="1" min="3" max="3"/>
+    <col width="49" customWidth="1" min="3" max="3"/>
     <col width="17" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="41" customWidth="1" min="6" max="6"/>
@@ -553,6 +553,87 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>&lt;20641191.1075855687472.JavaMail.evans@thyme&gt;</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Tue, 17 Oct 2000 02:26:00 -0700 (PDT)</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>phillip.allen@enron.com</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>Phillip K Allen</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>enron</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>Re: High Speed Internet Access</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>1. login:  pallen pw: ke9davis
+ I don't think these are required by the ISP 
+  2.  static IP address
+ IP: 64.216.90.105
+ Sub: 255.255.255.248
+ gate: 64.216.90.110
+ DNS: 151.164.1.8
+  3.  Company: 0413
+        RC:  105891</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	&lt;SI2PR06MB50915CD790AC930831A23BC0F77F2@SI2PR06MB5091.apcprd06.prod.outlook.com&gt;</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>Wed, 09 Oct 2024 10:52:18 +0000</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>Krishnananda R &lt;krishnananda.r@alphanimble.com&gt;</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>alphanimble</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Introduction </t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>Hi, my name is R Krishnananda. You can use this mail address to communicate with me.
+(Please ignore mail from rkrishnananda2003@gmail.com)
+Thank you
+R Krishnananda</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>